<commit_message>
Fixed an error in the measurement spreadsheet
</commit_message>
<xml_diff>
--- a/Demand/InputData/RR_Expected_Demand_Units_QAQC_Measurement_Values.xlsx
+++ b/Demand/InputData/RR_Expected_Demand_Units_QAQC_Measurement_Values.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aprashar\Documents\Github\DWRAT_DataScraping\Demand\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0B17BA-CE5E-47EB-BEE7-8386B6CABB58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5A1E7C-26B2-4FD2-B533-22E633269BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{A297D415-07B9-4C85-9CA4-1CDE38BCAE7E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A297D415-07B9-4C85-9CA4-1CDE38BCAE7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -225,9 +225,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -265,7 +265,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -371,7 +371,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -513,7 +513,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -523,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D74595C-3C80-49F1-9743-437EE37EBB20}">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -825,39 +825,39 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
         <f>312575.3/325851</f>
         <v>0.95925837269181313</v>
       </c>
-      <c r="L6">
+      <c r="I6">
         <f>285472.2/325851</f>
         <v>0.87608201294456678</v>
       </c>
-      <c r="M6">
+      <c r="J6">
         <f>137489.5/325851</f>
         <v>0.421939782293134</v>
       </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
         <f>36/325851</f>
         <v>1.1047994328696244E-4</v>
       </c>
-      <c r="Q6">
+      <c r="N6">
         <f>86.6/325851</f>
         <v>2.6576564135141517E-4</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -876,7 +876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8454921-0774-4A5A-8073-A67DDB7F796C}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated the QAQC script to perform corrections differently for calendar years and water years
</commit_message>
<xml_diff>
--- a/Demand/InputData/RR_Expected_Demand_Units_QAQC_Measurement_Values.xlsx
+++ b/Demand/InputData/RR_Expected_Demand_Units_QAQC_Measurement_Values.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aprashar\Documents\Github\DWRAT_DataScraping\Demand\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5A1E7C-26B2-4FD2-B533-22E633269BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E63AA2-44B6-441C-9EA4-A7DC97B343CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A297D415-07B9-4C85-9CA4-1CDE38BCAE7E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>APPLICATION_NUMBER</t>
   </si>
@@ -521,11 +521,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D74595C-3C80-49F1-9743-437EE37EBB20}">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -810,7 +808,7 @@
         <v>542161</v>
       </c>
       <c r="C6">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>28</v>
@@ -818,46 +816,63 @@
       <c r="E6" t="s">
         <v>7</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>542161</v>
+      </c>
+      <c r="C7">
+        <v>2022</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <f>312575.3/325851</f>
         <v>0.95925837269181313</v>
       </c>
-      <c r="I6">
+      <c r="I7">
         <f>285472.2/325851</f>
         <v>0.87608201294456678</v>
       </c>
-      <c r="J6">
+      <c r="J7">
         <f>137489.5/325851</f>
         <v>0.421939782293134</v>
       </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
         <f>36/325851</f>
         <v>1.1047994328696244E-4</v>
       </c>
-      <c r="N6">
+      <c r="N7">
         <f>86.6/325851</f>
         <v>2.6576564135141517E-4</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -866,7 +881,8 @@
     <hyperlink ref="D3" r:id="rId2" xr:uid="{B0809C65-4C2D-4D54-BD27-7BEDA437C4BB}"/>
     <hyperlink ref="D4" r:id="rId3" xr:uid="{6B906F1F-D381-4B34-AC01-60040EBD7609}"/>
     <hyperlink ref="D5" r:id="rId4" xr:uid="{29D3BC41-8870-4EAF-9321-7A75B185DE02}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{961372EA-BEEF-491F-9E47-1FEBDE35F8F9}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{961372EA-BEEF-491F-9E47-1FEBDE35F8F9}"/>
+    <hyperlink ref="D6" r:id="rId6" xr:uid="{69481C40-CA9A-4347-86FC-F3FB87A46C27}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>